<commit_message>
With Power BI Visual Day 1
</commit_message>
<xml_diff>
--- a/data/2020_2023_change_city.xlsx
+++ b/data/2020_2023_change_city.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\vol05\CBA\CBER\allusers\SDC\News\Posts\2024_09_06_Subcounty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/384aa62402beba2a/Documents/DA15/Capstone Project/tennessee_population_after_covid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C882C7-8D7A-45CC-BBAC-B6F36F05658B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="21600" windowHeight="11232" tabRatio="696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TN Municipalities and Locales" sheetId="8" r:id="rId1"/>
@@ -2566,22 +2566,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912D683C-ABC9-4C23-9765-896A08947408}">
   <dimension ref="A1:J353"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="20" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2613,7 +2615,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>229</v>
       </c>
@@ -2645,7 +2647,7 @@
         <v>-2.7722198057126288E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>207</v>
       </c>
@@ -2677,7 +2679,7 @@
         <v>-2.6110433311031526E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>170</v>
       </c>
@@ -2709,7 +2711,7 @@
         <v>3.5080388203462071E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -2741,7 +2743,7 @@
         <v>3.0082393373281637E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -2773,7 +2775,7 @@
         <v>7.8843524825531766E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>227</v>
       </c>
@@ -2805,7 +2807,7 @@
         <v>7.5918494767717892E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -2837,7 +2839,7 @@
         <v>5.2332628276730755E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>163</v>
       </c>
@@ -2869,7 +2871,7 @@
         <v>3.115816706739219E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>158</v>
       </c>
@@ -2901,7 +2903,7 @@
         <v>9.53093153858561E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -2933,7 +2935,7 @@
         <v>2.4131103205138525E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>309</v>
       </c>
@@ -2965,7 +2967,7 @@
         <v>0.12344066739435522</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>298</v>
       </c>
@@ -2997,7 +2999,7 @@
         <v>7.3333956444527532E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>167</v>
       </c>
@@ -3029,7 +3031,7 @@
         <v>2.3131608386561295E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -3061,7 +3063,7 @@
         <v>-2.8437662562857638E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -3093,7 +3095,7 @@
         <v>-3.1169033565153022E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -3125,7 +3127,7 @@
         <v>0.12331853570392844</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -3157,7 +3159,7 @@
         <v>2.4374973913769356E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>178</v>
       </c>
@@ -3189,7 +3191,7 @@
         <v>0.23709855750687819</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -3221,7 +3223,7 @@
         <v>0.12695961995249405</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -3253,7 +3255,7 @@
         <v>-3.8293096238913708E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>224</v>
       </c>
@@ -3285,7 +3287,7 @@
         <v>8.1288111676661792E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>125</v>
       </c>
@@ -3317,7 +3319,7 @@
         <v>-2.4279725702100852E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>176</v>
       </c>
@@ -3349,7 +3351,7 @@
         <v>2.2887551341995816E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -3381,7 +3383,7 @@
         <v>4.9171413034145225E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>243</v>
       </c>
@@ -3413,7 +3415,7 @@
         <v>6.1738992211095217E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>201</v>
       </c>
@@ -3445,7 +3447,7 @@
         <v>1.3529981564228353E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>219</v>
       </c>
@@ -3477,7 +3479,7 @@
         <v>5.3116797900262469E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -3509,7 +3511,7 @@
         <v>2.4684545487988818E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>111</v>
       </c>
@@ -3541,7 +3543,7 @@
         <v>8.4821239238305271E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>242</v>
       </c>
@@ -3573,7 +3575,7 @@
         <v>0.16184778996344301</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>99</v>
       </c>
@@ -3605,7 +3607,7 @@
         <v>-1.023075536325942E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -3637,7 +3639,7 @@
         <v>0.129595015576324</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>308</v>
       </c>
@@ -3669,7 +3671,7 @@
         <v>3.6639191704333954E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>199</v>
       </c>
@@ -3701,7 +3703,7 @@
         <v>8.2103546677537706E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>129</v>
       </c>
@@ -3733,7 +3735,7 @@
         <v>-2.0622611822881547E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>297</v>
       </c>
@@ -3765,7 +3767,7 @@
         <v>6.9416898056326851E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -3797,7 +3799,7 @@
         <v>-9.5521647438283099E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>293</v>
       </c>
@@ -3829,7 +3831,7 @@
         <v>6.3698311254073728E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>237</v>
       </c>
@@ -3861,7 +3863,7 @@
         <v>9.8562482208938235E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>344</v>
       </c>
@@ -3893,7 +3895,7 @@
         <v>0.17269321917284611</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -3925,7 +3927,7 @@
         <v>2.621697733673059E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>180</v>
       </c>
@@ -3957,7 +3959,7 @@
         <v>6.3132335087009314E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>101</v>
       </c>
@@ -3989,7 +3991,7 @@
         <v>-1.5691672401927047E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>174</v>
       </c>
@@ -4021,7 +4023,7 @@
         <v>8.4830339321357289E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>349</v>
       </c>
@@ -4053,7 +4055,7 @@
         <v>6.0812247501594724E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -4085,7 +4087,7 @@
         <v>4.4825874175473436E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -4117,7 +4119,7 @@
         <v>0.21708606856309262</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>171</v>
       </c>
@@ -4149,7 +4151,7 @@
         <v>4.3796925277082586E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>300</v>
       </c>
@@ -4181,7 +4183,7 @@
         <v>1.0691919963341989E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>168</v>
       </c>
@@ -4213,7 +4215,7 @@
         <v>4.3113571548397921E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>80</v>
       </c>
@@ -4245,7 +4247,7 @@
         <v>4.5792693007108615E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>143</v>
       </c>
@@ -4277,7 +4279,7 @@
         <v>5.4662655779974215E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>269</v>
       </c>
@@ -4309,7 +4311,7 @@
         <v>1.207952352990521E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>89</v>
       </c>
@@ -4341,7 +4343,7 @@
         <v>4.2850024912805179E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>179</v>
       </c>
@@ -4373,7 +4375,7 @@
         <v>0.15985790408525755</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>67</v>
       </c>
@@ -4405,7 +4407,7 @@
         <v>3.2292884771071333E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>213</v>
       </c>
@@ -4437,7 +4439,7 @@
         <v>8.3837429111531192E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -4469,7 +4471,7 @@
         <v>3.3383534136546184E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>200</v>
       </c>
@@ -4501,7 +4503,7 @@
         <v>1.6166281755196306E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -4533,7 +4535,7 @@
         <v>5.3086787951088579E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>85</v>
       </c>
@@ -4565,7 +4567,7 @@
         <v>4.2185730464326159E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>288</v>
       </c>
@@ -4597,7 +4599,7 @@
         <v>1.3586579786496604E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -4629,7 +4631,7 @@
         <v>2.7024341778440139E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>110</v>
       </c>
@@ -4661,7 +4663,7 @@
         <v>7.6987799747580979E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>198</v>
       </c>
@@ -4693,7 +4695,7 @@
         <v>3.4630350194552531E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>277</v>
       </c>
@@ -4725,7 +4727,7 @@
         <v>3.4134703615342266E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>294</v>
       </c>
@@ -4757,7 +4759,7 @@
         <v>6.5477534432151728E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>161</v>
       </c>
@@ -4789,7 +4791,7 @@
         <v>3.9511153298528716E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>318</v>
       </c>
@@ -4821,7 +4823,7 @@
         <v>0.1374784568474082</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>177</v>
       </c>
@@ -4853,7 +4855,7 @@
         <v>3.0245746691871456E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>328</v>
       </c>
@@ -4885,7 +4887,7 @@
         <v>2.9864652805021576E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>264</v>
       </c>
@@ -4917,7 +4919,7 @@
         <v>2.7935498523733816E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>109</v>
       </c>
@@ -4949,7 +4951,7 @@
         <v>2.4430871737923375E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>153</v>
       </c>
@@ -4981,7 +4983,7 @@
         <v>-4.5708481462671405E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>135</v>
       </c>
@@ -5013,7 +5015,7 @@
         <v>1.7019082001031461E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>132</v>
       </c>
@@ -5045,7 +5047,7 @@
         <v>1.4925373134328358E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>250</v>
       </c>
@@ -5077,7 +5079,7 @@
         <v>5.0529588961228259E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>210</v>
       </c>
@@ -5109,7 +5111,7 @@
         <v>1.4187866927592954E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>60</v>
       </c>
@@ -5141,7 +5143,7 @@
         <v>3.2847757783490431E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>144</v>
       </c>
@@ -5173,7 +5175,7 @@
         <v>1.375494071146245E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>234</v>
       </c>
@@ -5205,7 +5207,7 @@
         <v>1.6027976103744717E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>134</v>
       </c>
@@ -5237,7 +5239,7 @@
         <v>-8.6244070720137994E-4</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>226</v>
       </c>
@@ -5269,7 +5271,7 @@
         <v>6.8196202531645572E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>192</v>
       </c>
@@ -5301,7 +5303,7 @@
         <v>4.296754250386399E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>188</v>
       </c>
@@ -5333,7 +5335,7 @@
         <v>0.10406639004149378</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>314</v>
       </c>
@@ -5365,7 +5367,7 @@
         <v>3.1113876789047916E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>164</v>
       </c>
@@ -5397,7 +5399,7 @@
         <v>9.5890410958904104E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>235</v>
       </c>
@@ -5429,7 +5431,7 @@
         <v>1.0090090090090089E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>195</v>
       </c>
@@ -5461,7 +5463,7 @@
         <v>9.2140921409214101E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>212</v>
       </c>
@@ -5493,7 +5495,7 @@
         <v>-2.0595690747782004E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>181</v>
       </c>
@@ -5525,7 +5527,7 @@
         <v>4.4008550232616621E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>140</v>
       </c>
@@ -5557,7 +5559,7 @@
         <v>3.6794354838709679E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>106</v>
       </c>
@@ -5589,7 +5591,7 @@
         <v>-1.2368073878627968E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>315</v>
       </c>
@@ -5621,7 +5623,7 @@
         <v>3.4100596760443308E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -5653,7 +5655,7 @@
         <v>8.2028337061894108E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>141</v>
       </c>
@@ -5685,7 +5687,7 @@
         <v>1.3645667500568569E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>16</v>
       </c>
@@ -5717,7 +5719,7 @@
         <v>7.7338476374156223E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>77</v>
       </c>
@@ -5749,7 +5751,7 @@
         <v>1.1312217194570137E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>223</v>
       </c>
@@ -5781,7 +5783,7 @@
         <v>1.5722120658135285E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>205</v>
       </c>
@@ -5813,7 +5815,7 @@
         <v>7.1345482745250099E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>263</v>
       </c>
@@ -5845,7 +5847,7 @@
         <v>0.12551271534044298</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>197</v>
       </c>
@@ -5877,7 +5879,7 @@
         <v>-5.7979417306856069E-4</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>112</v>
       </c>
@@ -5909,7 +5911,7 @@
         <v>-2.1240441801189465E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>36</v>
       </c>
@@ -5941,7 +5943,7 @@
         <v>-1.0213914048949701E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>305</v>
       </c>
@@ -5973,7 +5975,7 @@
         <v>-1.7196560687862426E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>225</v>
       </c>
@@ -6005,7 +6007,7 @@
         <v>3.7453183520599251E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>72</v>
       </c>
@@ -6037,7 +6039,7 @@
         <v>4.6791443850267379E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>51</v>
       </c>
@@ -6069,7 +6071,7 @@
         <v>-2.7309968138370506E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>346</v>
       </c>
@@ -6101,7 +6103,7 @@
         <v>-3.277972027972028E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>154</v>
       </c>
@@ -6133,7 +6135,7 @@
         <v>1.4642937598558234E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>149</v>
       </c>
@@ -6165,7 +6167,7 @@
         <v>5.0472334682860998E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>114</v>
       </c>
@@ -6197,7 +6199,7 @@
         <v>-0.10741331207652451</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>241</v>
       </c>
@@ -6229,7 +6231,7 @@
         <v>-8.5556011489536316E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>291</v>
       </c>
@@ -6261,7 +6263,7 @@
         <v>-3.3036009250082591E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>189</v>
       </c>
@@ -6293,7 +6295,7 @@
         <v>-8.8919288645690833E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>184</v>
       </c>
@@ -6325,7 +6327,7 @@
         <v>3.0875223271242664E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>343</v>
       </c>
@@ -6357,7 +6359,7 @@
         <v>7.4360960495739731E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>331</v>
       </c>
@@ -6389,7 +6391,7 @@
         <v>-1.8370821758222064E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>324</v>
       </c>
@@ -6421,7 +6423,7 @@
         <v>-3.39943342776204E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>183</v>
       </c>
@@ -6453,7 +6455,7 @@
         <v>9.8492462311557782E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>302</v>
       </c>
@@ -6485,7 +6487,7 @@
         <v>6.0402684563758392E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>330</v>
       </c>
@@ -6517,7 +6519,7 @@
         <v>-1.5690376569037657E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>194</v>
       </c>
@@ -6549,7 +6551,7 @@
         <v>4.0606060606060604E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -6581,7 +6583,7 @@
         <v>4.1361845807540799E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>279</v>
       </c>
@@ -6613,7 +6615,7 @@
         <v>-6.4336264207591675E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>209</v>
       </c>
@@ -6645,7 +6647,7 @@
         <v>8.9802130898021304E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>160</v>
       </c>
@@ -6677,7 +6679,7 @@
         <v>1.3827433628318584E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>84</v>
       </c>
@@ -6709,7 +6711,7 @@
         <v>7.6808573980351291E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>159</v>
       </c>
@@ -6741,7 +6743,7 @@
         <v>2.7709054923305294E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>301</v>
       </c>
@@ -6773,7 +6775,7 @@
         <v>2.8896672504378284E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>185</v>
       </c>
@@ -6805,7 +6807,7 @@
         <v>5.1031487513572206E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>245</v>
       </c>
@@ -6837,7 +6839,7 @@
         <v>2.8450363196125907E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>329</v>
       </c>
@@ -6869,7 +6871,7 @@
         <v>2.0303030303030302E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>230</v>
       </c>
@@ -6901,7 +6903,7 @@
         <v>-1.7996400719856028E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>25</v>
       </c>
@@ -6933,7 +6935,7 @@
         <v>3.6099865047233469E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>304</v>
       </c>
@@ -6965,7 +6967,7 @@
         <v>-3.9070067807555696E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>93</v>
       </c>
@@ -6997,7 +6999,7 @@
         <v>-1.7958097771865647E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>40</v>
       </c>
@@ -7029,7 +7031,7 @@
         <v>-6.9372181755116198E-4</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>351</v>
       </c>
@@ -7061,7 +7063,7 @@
         <v>4.6656869948567228E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>257</v>
       </c>
@@ -7093,7 +7095,7 @@
         <v>-6.873925949070458E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>342</v>
       </c>
@@ -7125,7 +7127,7 @@
         <v>2.0902090209020903E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>169</v>
       </c>
@@ -7157,7 +7159,7 @@
         <v>-1.35087095627444E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>217</v>
       </c>
@@ -7189,7 +7191,7 @@
         <v>-7.27802037845706E-4</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>259</v>
       </c>
@@ -7221,7 +7223,7 @@
         <v>0.16760746851932262</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>28</v>
       </c>
@@ -7253,7 +7255,7 @@
         <v>-0.10242214532871972</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>204</v>
       </c>
@@ -7285,7 +7287,7 @@
         <v>4.4939271255060725E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>345</v>
       </c>
@@ -7317,7 +7319,7 @@
         <v>9.8193244304791826E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>221</v>
       </c>
@@ -7349,7 +7351,7 @@
         <v>2.2508038585209004E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>29</v>
       </c>
@@ -7381,7 +7383,7 @@
         <v>5.6887444128403087E-3</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>222</v>
       </c>
@@ -7413,7 +7415,7 @@
         <v>1.8189334435717238E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>88</v>
       </c>
@@ -7445,7 +7447,7 @@
         <v>2.9052631578947368E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>157</v>
       </c>
@@ -7477,7 +7479,7 @@
         <v>-8.6994345367551115E-3</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>8</v>
       </c>
@@ -7509,7 +7511,7 @@
         <v>4.288164665523156E-4</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>96</v>
       </c>
@@ -7541,7 +7543,7 @@
         <v>6.0684872128305162E-3</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>119</v>
       </c>
@@ -7573,7 +7575,7 @@
         <v>4.4276457883369327E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>76</v>
       </c>
@@ -7605,7 +7607,7 @@
         <v>-1.0737790093522688E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>7</v>
       </c>
@@ -7637,7 +7639,7 @@
         <v>6.18921308576481E-3</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>107</v>
       </c>
@@ -7669,7 +7671,7 @@
         <v>1.3233348037053375E-3</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>55</v>
       </c>
@@ -7701,7 +7703,7 @@
         <v>1.1341083073433513E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>350</v>
       </c>
@@ -7733,7 +7735,7 @@
         <v>3.611971104231166E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>303</v>
       </c>
@@ -7765,7 +7767,7 @@
         <v>-1.8758374274229567E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>266</v>
       </c>
@@ -7797,7 +7799,7 @@
         <v>-1.205682225140265E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>261</v>
       </c>
@@ -7829,7 +7831,7 @@
         <v>5.3268765133171914E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>34</v>
       </c>
@@ -7861,7 +7863,7 @@
         <v>2.6884301488238119E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>273</v>
       </c>
@@ -7893,7 +7895,7 @@
         <v>1.3295346628679962E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>162</v>
       </c>
@@ -7925,7 +7927,7 @@
         <v>-7.9106561191251753E-3</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>12</v>
       </c>
@@ -7957,7 +7959,7 @@
         <v>6.1151079136690649E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>13</v>
       </c>
@@ -7989,7 +7991,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>186</v>
       </c>
@@ -8021,7 +8023,7 @@
         <v>-2.9140359397765905E-3</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>139</v>
       </c>
@@ -8053,7 +8055,7 @@
         <v>-1.6794625719769675E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>254</v>
       </c>
@@ -8085,7 +8087,7 @@
         <v>-1.5965166908563134E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>290</v>
       </c>
@@ -8117,7 +8119,7 @@
         <v>5.3835800807537013E-3</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>335</v>
       </c>
@@ -8149,7 +8151,7 @@
         <v>-2.5201612903225806E-3</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>246</v>
       </c>
@@ -8181,7 +8183,7 @@
         <v>6.0654008438818562E-3</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -8213,7 +8215,7 @@
         <v>3.9142091152815014E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>24</v>
       </c>
@@ -8245,7 +8247,7 @@
         <v>0.22018927444794953</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>313</v>
       </c>
@@ -8277,7 +8279,7 @@
         <v>1.863684771033014E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>319</v>
       </c>
@@ -8309,7 +8311,7 @@
         <v>1.0052910052910053E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>79</v>
       </c>
@@ -8341,7 +8343,7 @@
         <v>6.1693774537296693E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>258</v>
       </c>
@@ -8373,7 +8375,7 @@
         <v>3.0136986301369864E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>90</v>
       </c>
@@ -8405,7 +8407,7 @@
         <v>2.2355507088331516E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>56</v>
       </c>
@@ -8437,7 +8439,7 @@
         <v>7.3537927041111756E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>31</v>
       </c>
@@ -8469,7 +8471,7 @@
         <v>-0.12255603242727706</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>35</v>
       </c>
@@ -8501,7 +8503,7 @@
         <v>1.0995052226498075E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>83</v>
       </c>
@@ -8533,7 +8535,7 @@
         <v>-1.8927444794952682E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>47</v>
       </c>
@@ -8565,7 +8567,7 @@
         <v>2.6548672566371681E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -8597,7 +8599,7 @@
         <v>3.8018433179723504E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>137</v>
       </c>
@@ -8629,7 +8631,7 @@
         <v>2.4698449167145319E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>274</v>
       </c>
@@ -8661,7 +8663,7 @@
         <v>-2.0046260601387818E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>26</v>
       </c>
@@ -8693,7 +8695,7 @@
         <v>3.9170506912442393E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>289</v>
       </c>
@@ -8725,7 +8727,7 @@
         <v>1.9585253456221197E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>58</v>
       </c>
@@ -8757,7 +8759,7 @@
         <v>2.9535864978902954E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>334</v>
       </c>
@@ -8789,7 +8791,7 @@
         <v>5.1767676767676768E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>278</v>
       </c>
@@ -8821,7 +8823,7 @@
         <v>3.6719706242350062E-3</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>86</v>
       </c>
@@ -8853,7 +8855,7 @@
         <v>3.8216560509554139E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>239</v>
       </c>
@@ -8885,7 +8887,7 @@
         <v>9.3457943925233638E-3</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>150</v>
       </c>
@@ -8917,7 +8919,7 @@
         <v>2.1929824561403508E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>347</v>
       </c>
@@ -8949,7 +8951,7 @@
         <v>-1.8270401948842874E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>166</v>
       </c>
@@ -8981,7 +8983,7 @@
         <v>3.6105738233397806E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>339</v>
       </c>
@@ -9013,7 +9015,7 @@
         <v>3.215434083601286E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>253</v>
       </c>
@@ -9045,7 +9047,7 @@
         <v>5.7142857142857143E-3</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>103</v>
       </c>
@@ -9077,7 +9079,7 @@
         <v>5.0033806626098715E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>306</v>
       </c>
@@ -9109,7 +9111,7 @@
         <v>5.2667578659370724E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>311</v>
       </c>
@@ -9141,7 +9143,7 @@
         <v>2.9850746268656716E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>172</v>
       </c>
@@ -9173,7 +9175,7 @@
         <v>-2.2935779816513763E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>30</v>
       </c>
@@ -9205,7 +9207,7 @@
         <v>-4.7493403693931395E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>323</v>
       </c>
@@ -9237,7 +9239,7 @@
         <v>2.2808267997148968E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>327</v>
       </c>
@@ -9269,7 +9271,7 @@
         <v>-7.0521861777150916E-4</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>216</v>
       </c>
@@ -9301,7 +9303,7 @@
         <v>1.2265512265512266E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>130</v>
       </c>
@@ -9333,7 +9335,7 @@
         <v>7.2992700729927005E-3</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>233</v>
       </c>
@@ -9365,7 +9367,7 @@
         <v>2.7488855869242199E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>49</v>
       </c>
@@ -9397,7 +9399,7 @@
         <v>2.4496461622210124E-3</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>128</v>
       </c>
@@ -9429,7 +9431,7 @@
         <v>-1.4695077149155032E-3</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>202</v>
       </c>
@@ -9461,7 +9463,7 @@
         <v>5.9435364041604752E-3</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>299</v>
       </c>
@@ -9493,7 +9495,7 @@
         <v>6.4719810576164161E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>317</v>
       </c>
@@ -9525,7 +9527,7 @@
         <v>1.1278195488721804E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>282</v>
       </c>
@@ -9557,7 +9559,7 @@
         <v>7.5700227100681302E-3</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>74</v>
       </c>
@@ -9589,7 +9591,7 @@
         <v>7.0388349514563103E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>265</v>
       </c>
@@ -9621,7 +9623,7 @@
         <v>-1.3086989992301771E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>33</v>
       </c>
@@ -9653,7 +9655,7 @@
         <v>1.443298969072165E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>14</v>
       </c>
@@ -9685,7 +9687,7 @@
         <v>1.4925373134328358E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>270</v>
       </c>
@@ -9717,7 +9719,7 @@
         <v>7.4688796680497929E-3</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>133</v>
       </c>
@@ -9749,7 +9751,7 @@
         <v>7.8590785907859076E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>105</v>
       </c>
@@ -9781,7 +9783,7 @@
         <v>-3.2467532467532464E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>280</v>
       </c>
@@ -9813,7 +9815,7 @@
         <v>0.10626185958254269</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>307</v>
       </c>
@@ -9845,7 +9847,7 @@
         <v>3.089598352214212E-3</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>211</v>
       </c>
@@ -9877,7 +9879,7 @@
         <v>1.4652014652014652E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>286</v>
       </c>
@@ -9909,7 +9911,7 @@
         <v>9.7087378640776691E-3</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>190</v>
       </c>
@@ -9941,7 +9943,7 @@
         <v>4.4160942100098133E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>341</v>
       </c>
@@ -9973,7 +9975,7 @@
         <v>1.7278617710583153E-3</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>247</v>
       </c>
@@ -10005,7 +10007,7 @@
         <v>4.746835443037975E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>38</v>
       </c>
@@ -10037,7 +10039,7 @@
         <v>-8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>10</v>
       </c>
@@ -10069,7 +10071,7 @@
         <v>6.0975609756097563E-3</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>87</v>
       </c>
@@ -10101,7 +10103,7 @@
         <v>2.4906600249066002E-3</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>287</v>
       </c>
@@ -10133,7 +10135,7 @@
         <v>8.9285714285714281E-3</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>232</v>
       </c>
@@ -10165,7 +10167,7 @@
         <v>5.54016620498615E-4</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>231</v>
       </c>
@@ -10197,7 +10199,7 @@
         <v>-2.7327935222672066E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>19</v>
       </c>
@@ -10229,7 +10231,7 @@
         <v>1.2725344644750796E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>98</v>
       </c>
@@ -10261,7 +10263,7 @@
         <v>0.14320388349514562</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>336</v>
       </c>
@@ -10293,7 +10295,7 @@
         <v>3.5164835164835165E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>292</v>
       </c>
@@ -10325,7 +10327,7 @@
         <v>-1.0683760683760684E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>81</v>
       </c>
@@ -10357,7 +10359,7 @@
         <v>2.3230088495575223E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>117</v>
       </c>
@@ -10389,7 +10391,7 @@
         <v>2.1276595744680851E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>69</v>
       </c>
@@ -10421,7 +10423,7 @@
         <v>1.1160714285714286E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>57</v>
       </c>
@@ -10453,7 +10455,7 @@
         <v>2.0524515393386546E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>155</v>
       </c>
@@ -10485,7 +10487,7 @@
         <v>4.5095828635851182E-3</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>43</v>
       </c>
@@ -10517,7 +10519,7 @@
         <v>-1.9920318725099601E-3</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>146</v>
       </c>
@@ -10549,7 +10551,7 @@
         <v>3.4364261168384879E-3</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>283</v>
       </c>
@@ -10581,7 +10583,7 @@
         <v>3.8022813688212927E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>276</v>
       </c>
@@ -10613,7 +10615,7 @@
         <v>-3.6496350364963502E-3</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>151</v>
       </c>
@@ -10645,7 +10647,7 @@
         <v>-7.8431372549019607E-3</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>66</v>
       </c>
@@ -10677,7 +10679,7 @@
         <v>3.1806615776081425E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>325</v>
       </c>
@@ -10709,7 +10711,7 @@
         <v>1.2562814070351759E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>353</v>
       </c>
@@ -10741,7 +10743,7 @@
         <v>-1.7094017094017096E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>236</v>
       </c>
@@ -10773,7 +10775,7 @@
         <v>4.563233376792699E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>100</v>
       </c>
@@ -10805,7 +10807,7 @@
         <v>7.7619663648124193E-3</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>316</v>
       </c>
@@ -10837,7 +10839,7 @@
         <v>1.7015706806282723E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>218</v>
       </c>
@@ -10869,7 +10871,7 @@
         <v>5.4719562243502051E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>44</v>
       </c>
@@ -10901,7 +10903,7 @@
         <v>1.5936254980079681E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>32</v>
       </c>
@@ -10933,7 +10935,7 @@
         <v>1.3531799729364006E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>78</v>
       </c>
@@ -10965,7 +10967,7 @@
         <v>1.8080667593880391E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>156</v>
       </c>
@@ -10997,7 +10999,7 @@
         <v>-3.4462952326249283E-3</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>267</v>
       </c>
@@ -11029,7 +11031,7 @@
         <v>8.5470085470085479E-3</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>285</v>
       </c>
@@ -11061,7 +11063,7 @@
         <v>-3.3653846153846152E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>208</v>
       </c>
@@ -11093,7 +11095,7 @@
         <v>1.5197568389057751E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>337</v>
       </c>
@@ -11125,7 +11127,7 @@
         <v>1.2158054711246201E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>256</v>
       </c>
@@ -11157,7 +11159,7 @@
         <v>9.0460526315789477E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>123</v>
       </c>
@@ -11189,7 +11191,7 @@
         <v>-1.5060240963855422E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>6</v>
       </c>
@@ -11221,7 +11223,7 @@
         <v>5.1529790660225443E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>322</v>
       </c>
@@ -11253,7 +11255,7 @@
         <v>0.11191335740072202</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>116</v>
       </c>
@@ -11285,7 +11287,7 @@
         <v>4.9019607843137254E-3</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>326</v>
       </c>
@@ -11317,7 +11319,7 @@
         <v>-1.6544117647058824E-2</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>203</v>
       </c>
@@ -11349,7 +11351,7 @@
         <v>6.8965517241379309E-3</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>332</v>
       </c>
@@ -11381,7 +11383,7 @@
         <v>2.6455026455026454E-2</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>249</v>
       </c>
@@ -11413,7 +11415,7 @@
         <v>3.6363636363636362E-2</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>22</v>
       </c>
@@ -11445,7 +11447,7 @@
         <v>7.7946768060836502E-2</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>220</v>
       </c>
@@ -11477,7 +11479,7 @@
         <v>-8.8183421516754845E-3</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>108</v>
       </c>
@@ -11509,7 +11511,7 @@
         <v>4.5028142589118199E-2</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>48</v>
       </c>
@@ -11541,7 +11543,7 @@
         <v>3.7383177570093455E-2</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>255</v>
       </c>
@@ -11573,7 +11575,7 @@
         <v>4.3726235741444866E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>262</v>
       </c>
@@ -11605,7 +11607,7 @@
         <v>9.2081031307550652E-3</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>312</v>
       </c>
@@ -11637,7 +11639,7 @@
         <v>3.6468330134357005E-2</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>136</v>
       </c>
@@ -11669,7 +11671,7 @@
         <v>-7.3782587309394985E-3</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>102</v>
       </c>
@@ -11701,7 +11703,7 @@
         <v>-1.6605166051660517E-2</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>121</v>
       </c>
@@ -11733,7 +11735,7 @@
         <v>-3.7593984962406013E-3</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>92</v>
       </c>
@@ -11765,7 +11767,7 @@
         <v>5.8350100603621731E-2</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>214</v>
       </c>
@@ -11797,7 +11799,7 @@
         <v>1.782178217821782E-2</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>281</v>
       </c>
@@ -11829,7 +11831,7 @@
         <v>-1.3828867761452032E-2</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>244</v>
       </c>
@@ -11861,7 +11863,7 @@
         <v>-1.6129032258064516E-2</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>118</v>
       </c>
@@ -11893,7 +11895,7 @@
         <v>2.1141649048625794E-3</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>127</v>
       </c>
@@ -11925,7 +11927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>260</v>
       </c>
@@ -11957,7 +11959,7 @@
         <v>4.3572984749455342E-3</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>21</v>
       </c>
@@ -11989,7 +11991,7 @@
         <v>5.057471264367816E-2</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>53</v>
       </c>
@@ -12021,7 +12023,7 @@
         <v>-1.2702893436838392E-2</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>73</v>
       </c>
@@ -12053,7 +12055,7 @@
         <v>2.0361990950226245E-2</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>94</v>
       </c>
@@ -12085,7 +12087,7 @@
         <v>-1.5283842794759825E-2</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>147</v>
       </c>
@@ -12117,7 +12119,7 @@
         <v>1.3544018058690745E-2</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>272</v>
       </c>
@@ -12149,7 +12151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>284</v>
       </c>
@@ -12181,7 +12183,7 @@
         <v>1.4354066985645933E-2</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>27</v>
       </c>
@@ -12213,7 +12215,7 @@
         <v>1.6949152542372881E-2</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>138</v>
       </c>
@@ -12245,7 +12247,7 @@
         <v>1.4527845036319613E-2</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>165</v>
       </c>
@@ -12277,7 +12279,7 @@
         <v>-1.873536299765808E-2</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>310</v>
       </c>
@@ -12309,7 +12311,7 @@
         <v>-4.8192771084337354E-3</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>61</v>
       </c>
@@ -12341,7 +12343,7 @@
         <v>1.5915119363395226E-2</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>126</v>
       </c>
@@ -12373,7 +12375,7 @@
         <v>2.197802197802198E-2</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>45</v>
       </c>
@@ -12405,7 +12407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>91</v>
       </c>
@@ -12437,7 +12439,7 @@
         <v>4.9418604651162788E-2</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>338</v>
       </c>
@@ -12469,7 +12471,7 @@
         <v>2.564102564102564E-2</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>340</v>
       </c>
@@ -12501,7 +12503,7 @@
         <v>-6.7379182156133829E-3</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>182</v>
       </c>
@@ -12533,7 +12535,7 @@
         <v>2.1084337349397589E-2</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>352</v>
       </c>
@@ -12565,7 +12567,7 @@
         <v>-1.1661807580174927E-2</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>131</v>
       </c>
@@ -12597,7 +12599,7 @@
         <v>-5.8823529411764705E-3</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>348</v>
       </c>
@@ -12629,7 +12631,7 @@
         <v>-3.151862464183381E-2</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>268</v>
       </c>
@@ -12661,7 +12663,7 @@
         <v>3.0581039755351682E-3</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>82</v>
       </c>
@@ -12693,7 +12695,7 @@
         <v>3.2786885245901641E-2</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>54</v>
       </c>
@@ -12725,7 +12727,7 @@
         <v>5.016722408026756E-2</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>193</v>
       </c>
@@ -12757,7 +12759,7 @@
         <v>6.4846416382252553E-2</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>42</v>
       </c>
@@ -12789,7 +12791,7 @@
         <v>-3.8418194857084316E-2</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>52</v>
       </c>
@@ -12821,7 +12823,7 @@
         <v>-1.3157894736842105E-2</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>196</v>
       </c>
@@ -12853,7 +12855,7 @@
         <v>3.4482758620689655E-3</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>122</v>
       </c>
@@ -12885,7 +12887,7 @@
         <v>-3.4965034965034965E-3</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>251</v>
       </c>
@@ -12917,7 +12919,7 @@
         <v>3.5460992907801418E-3</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>20</v>
       </c>
@@ -12949,7 +12951,7 @@
         <v>2.5547445255474453E-2</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>50</v>
       </c>
@@ -12981,7 +12983,7 @@
         <v>-1.2647187091146969E-2</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>113</v>
       </c>
@@ -13013,7 +13015,7 @@
         <v>3.6496350364963502E-3</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>321</v>
       </c>
@@ -13045,7 +13047,7 @@
         <v>7.4906367041198503E-3</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>152</v>
       </c>
@@ -13077,7 +13079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>37</v>
       </c>
@@ -13109,7 +13111,7 @@
         <v>-2.7027027027027029E-2</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>275</v>
       </c>
@@ -13141,7 +13143,7 @@
         <v>-4.048582995951417E-3</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>271</v>
       </c>
@@ -13173,7 +13175,7 @@
         <v>-4.2161520190023755E-2</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>252</v>
       </c>
@@ -13205,7 +13207,7 @@
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>240</v>
       </c>
@@ -13237,7 +13239,7 @@
         <v>3.608247422680412E-2</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>64</v>
       </c>
@@ -13269,7 +13271,7 @@
         <v>-0.15022590361445784</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>206</v>
       </c>
@@ -13301,7 +13303,7 @@
         <v>1.0582010582010581E-2</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>104</v>
       </c>
@@ -13333,7 +13335,7 @@
         <v>5.4054054054054057E-3</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>296</v>
       </c>
@@ -13365,7 +13367,7 @@
         <v>3.4883720930232558E-2</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>215</v>
       </c>
@@ -13397,7 +13399,7 @@
         <v>-1.8633540372670808E-2</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>173</v>
       </c>
@@ -13429,7 +13431,7 @@
         <v>-2.4E-2</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>320</v>
       </c>
@@ -13461,7 +13463,7 @@
         <v>-0.1359979889391654</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>333</v>
       </c>
@@ -13493,7 +13495,7 @@
         <v>6.7961165048543687E-2</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>238</v>
       </c>
@@ -13525,7 +13527,7 @@
         <v>-9.2592592592592587E-3</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>295</v>
       </c>
@@ -13557,7 +13559,7 @@
         <v>-1.020408163265306E-2</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>248</v>
       </c>
@@ -13589,7 +13591,7 @@
         <v>-3.4090909090909088E-2</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>148</v>
       </c>
@@ -13621,7 +13623,7 @@
         <v>1.2658227848101266E-2</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>75</v>
       </c>
@@ -13653,27 +13655,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A352" s="2" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>716</v>
       </c>

</xml_diff>